<commit_message>
10 percent sample, no age/sex
</commit_message>
<xml_diff>
--- a/1_Data/GIVES21_example_data_dictionary.xlsx
+++ b/1_Data/GIVES21_example_data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/tmp/4-stages-IBD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/tmp/4-stages-IBD/1_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4266D8D-242D-D447-B935-49D22D364163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251DC0DF-E7C1-6848-9D4A-1563F6362548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67380" yWindow="-7860" windowWidth="28040" windowHeight="16940" xr2:uid="{10D29239-36C5-0D44-AA74-14C499623539}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12300" windowHeight="17500" xr2:uid="{10D29239-36C5-0D44-AA74-14C499623539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>COLUMN NAME</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>CALCULATIONS</t>
-  </si>
-  <si>
-    <t>index</t>
   </si>
   <si>
     <t>author</t>
@@ -77,14 +74,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>epi_stage</t>
-  </si>
-  <si>
-    <t>1 = Emergence
-2 = Acceleration in Incidence
-3 = Compounding Prevalence</t>
   </si>
   <si>
     <t>age</t>
@@ -151,30 +140,6 @@
     <t>Numerator of rate. Number of patients with undefined IBD</t>
   </si>
   <si>
-    <t>male_UC_patients</t>
-  </si>
-  <si>
-    <t>Sex-specific numerator. Number of male patients with ulcerative colitis.</t>
-  </si>
-  <si>
-    <t>male_CD_patients</t>
-  </si>
-  <si>
-    <t>Sex-specific numerator. Number of male patients with Crohn's disease.</t>
-  </si>
-  <si>
-    <t>female_UC_patients</t>
-  </si>
-  <si>
-    <t>Sex-specific numerator, Number of female patients with ulcerative colits.</t>
-  </si>
-  <si>
-    <t>female_CD_patients</t>
-  </si>
-  <si>
-    <t>Sex-specific numerator. Number of female patients with Crohn's disease.</t>
-  </si>
-  <si>
     <t>UC_rate</t>
   </si>
   <si>
@@ -194,18 +159,6 @@
   </si>
   <si>
     <t>=IF(AND(UC_IBDu_calculated = "", UC_IBDu_provided = ""), "", IF(UC_IBDu_calculated= "", UC_IBDu_provided, "UC_IBDu_calculated))</t>
-  </si>
-  <si>
-    <t>male_UC_rate</t>
-  </si>
-  <si>
-    <t>male_CD_rate</t>
-  </si>
-  <si>
-    <t>female_UC_rate</t>
-  </si>
-  <si>
-    <t>female_CD_rate</t>
   </si>
   <si>
     <t>notes</t>
@@ -228,9 +181,6 @@
     </r>
   </si>
   <si>
-    <t>master index</t>
-  </si>
-  <si>
     <t>unique identifier for each study included in review</t>
   </si>
   <si>
@@ -274,9 +224,6 @@
   </si>
   <si>
     <t>Type of rate</t>
-  </si>
-  <si>
-    <t>Region's epidemiological stage in the given year based on machine learning classifier (random forest approach)</t>
   </si>
 </sst>
 </file>
@@ -663,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B1EEB2-2BB8-394B-A391-D7AC97E2EE73}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,20 +640,20 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -716,37 +663,37 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -756,17 +703,17 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -777,261 +724,167 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D19" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="50" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" ht="50" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>